<commit_message>
Modified 'CSES FINAL dataset.csv' so that it agrees with the .xlsx version.
</commit_message>
<xml_diff>
--- a/tests/testdata/CSES FINAL dataset.xlsx
+++ b/tests/testdata/CSES FINAL dataset.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Amanda\Pusto\git\SingleCaseES\tests\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jepus\OneDrive\Documents\SingleCaseES\tests\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBD4DBA5-E986-482F-9336-FA485110CDD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC0BAD0C-C2E8-4347-B624-F07B779221EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{290A1585-F2DD-4BBD-AFEB-CD568743FE1B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{290A1585-F2DD-4BBD-AFEB-CD568743FE1B}"/>
   </bookViews>
   <sheets>
     <sheet name="ALL" sheetId="12" r:id="rId1"/>
@@ -117,6 +117,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="176" formatCode="0.000000000000000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -146,12 +149,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -471,22 +477,23 @@
   <dimension ref="A1:H328"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F156" sqref="F156"/>
+      <selection activeCell="E2" sqref="E2:E202"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="1"/>
-    <col min="2" max="2" width="12.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="10.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="14.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.21875" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="8.85546875" style="1"/>
+    <col min="2" max="2" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
@@ -512,7 +519,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>221</v>
       </c>
@@ -525,7 +532,7 @@
       <c r="D2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="3">
         <v>44.4</v>
       </c>
       <c r="F2" s="2">
@@ -538,7 +545,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>221</v>
       </c>
@@ -551,7 +558,7 @@
       <c r="D3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="3">
         <v>0.02</v>
       </c>
       <c r="F3" s="2">
@@ -564,7 +571,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>221</v>
       </c>
@@ -577,7 +584,7 @@
       <c r="D4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="3">
         <v>38.5</v>
       </c>
       <c r="F4" s="2">
@@ -590,7 +597,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>221</v>
       </c>
@@ -603,7 +610,7 @@
       <c r="D5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="3">
         <v>11.5</v>
       </c>
       <c r="F5" s="2">
@@ -616,7 +623,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>221</v>
       </c>
@@ -629,7 +636,7 @@
       <c r="D6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="3">
         <v>44.4</v>
       </c>
       <c r="F6" s="2">
@@ -642,7 +649,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>221</v>
       </c>
@@ -655,7 +662,7 @@
       <c r="D7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="3">
         <v>20.6</v>
       </c>
       <c r="F7" s="2">
@@ -668,7 +675,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>221</v>
       </c>
@@ -681,7 +688,7 @@
       <c r="D8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="3">
         <v>54.5</v>
       </c>
       <c r="F8" s="2">
@@ -694,7 +701,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>221</v>
       </c>
@@ -707,7 +714,7 @@
       <c r="D9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="3">
         <v>58.4</v>
       </c>
       <c r="F9" s="2">
@@ -720,7 +727,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>221</v>
       </c>
@@ -733,7 +740,7 @@
       <c r="D10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="3">
         <v>66.599999999999994</v>
       </c>
       <c r="F10" s="2">
@@ -746,7 +753,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>221</v>
       </c>
@@ -759,7 +766,7 @@
       <c r="D11" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="3">
         <v>46.8</v>
       </c>
       <c r="F11" s="2">
@@ -772,7 +779,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>221</v>
       </c>
@@ -785,7 +792,7 @@
       <c r="D12" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="3">
         <v>46.8</v>
       </c>
       <c r="F12" s="2">
@@ -798,7 +805,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>221</v>
       </c>
@@ -811,7 +818,7 @@
       <c r="D13" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="3">
         <v>20.7</v>
       </c>
       <c r="F13" s="2">
@@ -824,7 +831,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>221</v>
       </c>
@@ -837,7 +844,7 @@
       <c r="D14" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14" s="3">
         <v>18.899999999999999</v>
       </c>
       <c r="F14" s="2">
@@ -850,7 +857,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>221</v>
       </c>
@@ -863,7 +870,7 @@
       <c r="D15" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15" s="3">
         <v>47</v>
       </c>
       <c r="F15" s="2">
@@ -876,7 +883,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>221</v>
       </c>
@@ -889,7 +896,7 @@
       <c r="D16" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16" s="3">
         <v>58.6</v>
       </c>
       <c r="F16" s="2">
@@ -902,7 +909,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>221</v>
       </c>
@@ -915,7 +922,7 @@
       <c r="D17" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E17" s="2">
+      <c r="E17" s="3">
         <v>54.8</v>
       </c>
       <c r="F17" s="2">
@@ -928,7 +935,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>221</v>
       </c>
@@ -941,7 +948,7 @@
       <c r="D18" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E18" s="3">
         <v>58.8</v>
       </c>
       <c r="F18" s="2">
@@ -954,7 +961,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>221</v>
       </c>
@@ -967,7 +974,7 @@
       <c r="D19" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E19" s="2">
+      <c r="E19" s="3">
         <v>67.099999999999994</v>
       </c>
       <c r="F19" s="2">
@@ -980,7 +987,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>221</v>
       </c>
@@ -993,7 +1000,7 @@
       <c r="D20" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E20" s="2">
+      <c r="E20" s="3">
         <v>16.8</v>
       </c>
       <c r="F20" s="2">
@@ -1006,7 +1013,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>221</v>
       </c>
@@ -1019,7 +1026,7 @@
       <c r="D21" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E21" s="2">
+      <c r="E21" s="3">
         <v>41.3</v>
       </c>
       <c r="F21" s="2">
@@ -1032,7 +1039,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>221</v>
       </c>
@@ -1045,7 +1052,7 @@
       <c r="D22" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E22" s="2">
+      <c r="E22" s="3">
         <v>1</v>
       </c>
       <c r="F22" s="2">
@@ -1058,7 +1065,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>221</v>
       </c>
@@ -1071,7 +1078,7 @@
       <c r="D23" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E23" s="2">
+      <c r="E23" s="3">
         <v>51.2</v>
       </c>
       <c r="F23" s="2">
@@ -1084,7 +1091,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>221</v>
       </c>
@@ -1097,7 +1104,7 @@
       <c r="D24" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E24" s="2">
+      <c r="E24" s="3">
         <v>67.400000000000006</v>
       </c>
       <c r="F24" s="2">
@@ -1110,7 +1117,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>221</v>
       </c>
@@ -1123,7 +1130,7 @@
       <c r="D25" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E25" s="2">
+      <c r="E25" s="3">
         <v>99.3</v>
       </c>
       <c r="F25" s="2">
@@ -1136,7 +1143,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>221</v>
       </c>
@@ -1149,7 +1156,7 @@
       <c r="D26" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E26" s="2">
+      <c r="E26" s="3">
         <v>64</v>
       </c>
       <c r="F26" s="2">
@@ -1162,7 +1169,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>221</v>
       </c>
@@ -1175,7 +1182,7 @@
       <c r="D27" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E27" s="2">
+      <c r="E27" s="3">
         <v>99.1</v>
       </c>
       <c r="F27" s="2">
@@ -1188,7 +1195,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>221</v>
       </c>
@@ -1201,7 +1208,7 @@
       <c r="D28" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E28" s="2">
+      <c r="E28" s="3">
         <v>99.8</v>
       </c>
       <c r="F28" s="2">
@@ -1214,7 +1221,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>221</v>
       </c>
@@ -1227,7 +1234,7 @@
       <c r="D29" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E29" s="2">
+      <c r="E29" s="3">
         <v>99.3</v>
       </c>
       <c r="F29" s="2">
@@ -1240,7 +1247,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>221</v>
       </c>
@@ -1253,7 +1260,7 @@
       <c r="D30" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E30" s="2">
+      <c r="E30" s="3">
         <v>45.3</v>
       </c>
       <c r="F30" s="2">
@@ -1266,7 +1273,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>221</v>
       </c>
@@ -1279,7 +1286,7 @@
       <c r="D31" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E31" s="2">
+      <c r="E31" s="3">
         <v>84.5</v>
       </c>
       <c r="F31" s="2">
@@ -1292,7 +1299,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>221</v>
       </c>
@@ -1305,7 +1312,7 @@
       <c r="D32" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E32" s="2">
+      <c r="E32" s="3">
         <v>65.5</v>
       </c>
       <c r="F32" s="2">
@@ -1318,7 +1325,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>221</v>
       </c>
@@ -1331,7 +1338,7 @@
       <c r="D33" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E33" s="2">
+      <c r="E33" s="3">
         <v>26.1</v>
       </c>
       <c r="F33" s="2">
@@ -1344,7 +1351,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>221</v>
       </c>
@@ -1357,7 +1364,7 @@
       <c r="D34" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E34" s="2">
+      <c r="E34" s="3">
         <v>24.4</v>
       </c>
       <c r="F34" s="2">
@@ -1370,7 +1377,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>221</v>
       </c>
@@ -1383,7 +1390,7 @@
       <c r="D35" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E35" s="2">
+      <c r="E35" s="3">
         <v>92</v>
       </c>
       <c r="F35" s="2">
@@ -1396,7 +1403,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>221</v>
       </c>
@@ -1409,7 +1416,7 @@
       <c r="D36" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E36" s="2">
+      <c r="E36" s="3">
         <v>100</v>
       </c>
       <c r="F36" s="2">
@@ -1422,7 +1429,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>221</v>
       </c>
@@ -1435,7 +1442,7 @@
       <c r="D37" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E37" s="2">
+      <c r="E37" s="3">
         <v>74</v>
       </c>
       <c r="F37" s="2">
@@ -1448,7 +1455,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>221</v>
       </c>
@@ -1461,7 +1468,7 @@
       <c r="D38" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E38" s="2">
+      <c r="E38" s="3">
         <v>4.4000000000000004</v>
       </c>
       <c r="F38" s="2">
@@ -1474,7 +1481,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>221</v>
       </c>
@@ -1487,7 +1494,7 @@
       <c r="D39" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E39" s="2">
+      <c r="E39" s="3">
         <v>4.9000000000000004</v>
       </c>
       <c r="F39" s="2">
@@ -1500,7 +1507,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>221</v>
       </c>
@@ -1513,7 +1520,7 @@
       <c r="D40" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E40" s="2">
+      <c r="E40" s="3">
         <v>0</v>
       </c>
       <c r="F40" s="2">
@@ -1526,7 +1533,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>221</v>
       </c>
@@ -1539,7 +1546,7 @@
       <c r="D41" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E41" s="2">
+      <c r="E41" s="3">
         <v>49.5</v>
       </c>
       <c r="F41" s="2">
@@ -1552,7 +1559,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>221</v>
       </c>
@@ -1565,7 +1572,7 @@
       <c r="D42" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E42" s="2">
+      <c r="E42" s="3">
         <v>44.1</v>
       </c>
       <c r="F42" s="2">
@@ -1578,7 +1585,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>221</v>
       </c>
@@ -1591,7 +1598,7 @@
       <c r="D43" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E43" s="2">
+      <c r="E43" s="3">
         <v>54.9</v>
       </c>
       <c r="F43" s="2">
@@ -1604,7 +1611,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>221</v>
       </c>
@@ -1617,7 +1624,7 @@
       <c r="D44" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E44" s="2">
+      <c r="E44" s="3">
         <v>72.3</v>
       </c>
       <c r="F44" s="2">
@@ -1630,7 +1637,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>221</v>
       </c>
@@ -1643,7 +1650,7 @@
       <c r="D45" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E45" s="2">
+      <c r="E45" s="3">
         <v>100</v>
       </c>
       <c r="F45" s="2">
@@ -1656,7 +1663,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>221</v>
       </c>
@@ -1669,7 +1676,7 @@
       <c r="D46" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E46" s="2">
+      <c r="E46" s="3">
         <v>62.1</v>
       </c>
       <c r="F46" s="2">
@@ -1682,7 +1689,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>221</v>
       </c>
@@ -1695,7 +1702,7 @@
       <c r="D47" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E47" s="2">
+      <c r="E47" s="3">
         <v>71.400000000000006</v>
       </c>
       <c r="F47" s="2">
@@ -1708,7 +1715,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>221</v>
       </c>
@@ -1721,7 +1728,7 @@
       <c r="D48" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E48" s="2">
+      <c r="E48" s="3">
         <v>10.9</v>
       </c>
       <c r="F48" s="2">
@@ -1734,7 +1741,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>221</v>
       </c>
@@ -1747,7 +1754,7 @@
       <c r="D49" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E49" s="2">
+      <c r="E49" s="3">
         <v>0</v>
       </c>
       <c r="F49" s="2">
@@ -1760,7 +1767,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>221</v>
       </c>
@@ -1773,7 +1780,7 @@
       <c r="D50" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E50" s="2">
+      <c r="E50" s="3">
         <v>0</v>
       </c>
       <c r="F50" s="2">
@@ -1786,7 +1793,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>221</v>
       </c>
@@ -1799,7 +1806,7 @@
       <c r="D51" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E51" s="2">
+      <c r="E51" s="3">
         <v>60.1</v>
       </c>
       <c r="F51" s="2">
@@ -1812,7 +1819,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>221</v>
       </c>
@@ -1825,7 +1832,7 @@
       <c r="D52" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E52" s="2">
+      <c r="E52" s="3">
         <v>56.1</v>
       </c>
       <c r="F52" s="2">
@@ -1838,7 +1845,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>221</v>
       </c>
@@ -1851,7 +1858,7 @@
       <c r="D53" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E53" s="2">
+      <c r="E53" s="3">
         <v>75</v>
       </c>
       <c r="F53" s="2">
@@ -1864,7 +1871,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>221</v>
       </c>
@@ -1877,7 +1884,7 @@
       <c r="D54" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E54" s="2">
+      <c r="E54" s="3">
         <v>62</v>
       </c>
       <c r="F54" s="2">
@@ -1890,7 +1897,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>221</v>
       </c>
@@ -1903,7 +1910,7 @@
       <c r="D55" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E55" s="2">
+      <c r="E55" s="3">
         <v>82.2</v>
       </c>
       <c r="F55" s="2">
@@ -1916,7 +1923,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>120</v>
       </c>
@@ -1929,7 +1936,7 @@
       <c r="D56" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E56" s="2">
+      <c r="E56" s="3">
         <v>0.19512195121951217</v>
       </c>
       <c r="F56" s="2">
@@ -1942,7 +1949,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>120</v>
       </c>
@@ -1955,7 +1962,7 @@
       <c r="D57" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E57" s="2">
+      <c r="E57" s="3">
         <v>0.41025641025641024</v>
       </c>
       <c r="F57" s="2">
@@ -1968,7 +1975,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>120</v>
       </c>
@@ -1981,7 +1988,7 @@
       <c r="D58" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E58" s="2">
+      <c r="E58" s="3">
         <v>0.29032258064516125</v>
       </c>
       <c r="F58" s="2">
@@ -1994,7 +2001,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>120</v>
       </c>
@@ -2007,7 +2014,7 @@
       <c r="D59" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E59" s="2">
+      <c r="E59" s="3">
         <v>0.5</v>
       </c>
       <c r="F59" s="2">
@@ -2020,7 +2027,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>120</v>
       </c>
@@ -2033,7 +2040,7 @@
       <c r="D60" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E60" s="2">
+      <c r="E60" s="3">
         <v>0.6216216216216216</v>
       </c>
       <c r="F60" s="2">
@@ -2046,7 +2053,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>120</v>
       </c>
@@ -2059,7 +2066,7 @@
       <c r="D61" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E61" s="2">
+      <c r="E61" s="3">
         <v>0.51428571428571435</v>
       </c>
       <c r="F61" s="2">
@@ -2072,7 +2079,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>120</v>
       </c>
@@ -2085,7 +2092,7 @@
       <c r="D62" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E62" s="2">
+      <c r="E62" s="3">
         <v>0.28260869565217389</v>
       </c>
       <c r="F62" s="2">
@@ -2098,7 +2105,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>120</v>
       </c>
@@ -2111,7 +2118,7 @@
       <c r="D63" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E63" s="2">
+      <c r="E63" s="3">
         <v>0.37037037037037035</v>
       </c>
       <c r="F63" s="2">
@@ -2124,7 +2131,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>120</v>
       </c>
@@ -2137,7 +2144,7 @@
       <c r="D64" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E64" s="2">
+      <c r="E64" s="3">
         <v>0.63888888888888895</v>
       </c>
       <c r="F64" s="2">
@@ -2150,7 +2157,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>120</v>
       </c>
@@ -2163,7 +2170,7 @@
       <c r="D65" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E65" s="2">
+      <c r="E65" s="3">
         <v>0.5714285714285714</v>
       </c>
       <c r="F65" s="2">
@@ -2176,7 +2183,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>120</v>
       </c>
@@ -2189,7 +2196,7 @@
       <c r="D66" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E66" s="2">
+      <c r="E66" s="3">
         <v>0.58139534883720934</v>
       </c>
       <c r="F66" s="2">
@@ -2202,7 +2209,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>120</v>
       </c>
@@ -2215,7 +2222,7 @@
       <c r="D67" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E67" s="2">
+      <c r="E67" s="3">
         <v>0.69444444444444442</v>
       </c>
       <c r="F67" s="2">
@@ -2228,7 +2235,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>120</v>
       </c>
@@ -2241,7 +2248,7 @@
       <c r="D68" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E68" s="2">
+      <c r="E68" s="3">
         <v>0.60526315789473684</v>
       </c>
       <c r="F68" s="2">
@@ -2254,7 +2261,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>120</v>
       </c>
@@ -2267,7 +2274,7 @@
       <c r="D69" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E69" s="2">
+      <c r="E69" s="3">
         <v>0.58139534883720934</v>
       </c>
       <c r="F69" s="2">
@@ -2280,7 +2287,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>120</v>
       </c>
@@ -2293,7 +2300,7 @@
       <c r="D70" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E70" s="2">
+      <c r="E70" s="3">
         <v>0.6470588235294118</v>
       </c>
       <c r="F70" s="2">
@@ -2306,7 +2313,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>120</v>
       </c>
@@ -2319,7 +2326,7 @@
       <c r="D71" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E71" s="2">
+      <c r="E71" s="3">
         <v>0.78787878787878785</v>
       </c>
       <c r="F71" s="2">
@@ -2332,7 +2339,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>120</v>
       </c>
@@ -2345,7 +2352,7 @@
       <c r="D72" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E72" s="2">
+      <c r="E72" s="3">
         <v>0.58823529411764708</v>
       </c>
       <c r="F72" s="2">
@@ -2358,7 +2365,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>120</v>
       </c>
@@ -2371,7 +2378,7 @@
       <c r="D73" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E73" s="2">
+      <c r="E73" s="3">
         <v>0.44444444444444448</v>
       </c>
       <c r="F73" s="2">
@@ -2384,7 +2391,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>120</v>
       </c>
@@ -2397,7 +2404,7 @@
       <c r="D74" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E74" s="2">
+      <c r="E74" s="3">
         <v>0.68421052631578949</v>
       </c>
       <c r="F74" s="2">
@@ -2410,7 +2417,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>120</v>
       </c>
@@ -2423,7 +2430,7 @@
       <c r="D75" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E75" s="2">
+      <c r="E75" s="3">
         <v>0.82352941176470595</v>
       </c>
       <c r="F75" s="2">
@@ -2436,7 +2443,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>120</v>
       </c>
@@ -2449,7 +2456,7 @@
       <c r="D76" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E76" s="2">
+      <c r="E76" s="3">
         <v>0.96969696969696972</v>
       </c>
       <c r="F76" s="2">
@@ -2462,7 +2469,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>120</v>
       </c>
@@ -2475,7 +2482,7 @@
       <c r="D77" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E77" s="2">
+      <c r="E77" s="3">
         <v>0.97222222222222221</v>
       </c>
       <c r="F77" s="2">
@@ -2488,7 +2495,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>120</v>
       </c>
@@ -2501,7 +2508,7 @@
       <c r="D78" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E78" s="2">
+      <c r="E78" s="3">
         <v>0.94285714285714284</v>
       </c>
       <c r="F78" s="2">
@@ -2514,7 +2521,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>120</v>
       </c>
@@ -2527,7 +2534,7 @@
       <c r="D79" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E79" s="2">
+      <c r="E79" s="3">
         <v>0.97368421052631582</v>
       </c>
       <c r="F79" s="2">
@@ -2540,7 +2547,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>120</v>
       </c>
@@ -2553,7 +2560,7 @@
       <c r="D80" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E80" s="2">
+      <c r="E80" s="3">
         <v>0.95744680851063824</v>
       </c>
       <c r="F80" s="2">
@@ -2566,7 +2573,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>120</v>
       </c>
@@ -2579,7 +2586,7 @@
       <c r="D81" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E81" s="2">
+      <c r="E81" s="3">
         <v>0.3125</v>
       </c>
       <c r="F81" s="2">
@@ -2592,7 +2599,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>120</v>
       </c>
@@ -2605,7 +2612,7 @@
       <c r="D82" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E82" s="2">
+      <c r="E82" s="3">
         <v>0.30232558139534887</v>
       </c>
       <c r="F82" s="2">
@@ -2618,7 +2625,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>120</v>
       </c>
@@ -2631,7 +2638,7 @@
       <c r="D83" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E83" s="2">
+      <c r="E83" s="3">
         <v>0.21212121212121213</v>
       </c>
       <c r="F83" s="2">
@@ -2644,7 +2651,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>120</v>
       </c>
@@ -2657,7 +2664,7 @@
       <c r="D84" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E84" s="2">
+      <c r="E84" s="3">
         <v>0.45945945945945948</v>
       </c>
       <c r="F84" s="2">
@@ -2670,7 +2677,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>120</v>
       </c>
@@ -2683,7 +2690,7 @@
       <c r="D85" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E85" s="2">
+      <c r="E85" s="3">
         <v>0.3658536585365853</v>
       </c>
       <c r="F85" s="2">
@@ -2696,7 +2703,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>120</v>
       </c>
@@ -2709,7 +2716,7 @@
       <c r="D86" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E86" s="2">
+      <c r="E86" s="3">
         <v>0.44186046511627908</v>
       </c>
       <c r="F86" s="2">
@@ -2722,7 +2729,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>120</v>
       </c>
@@ -2735,7 +2742,7 @@
       <c r="D87" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E87" s="2">
+      <c r="E87" s="3">
         <v>0.37499999999999994</v>
       </c>
       <c r="F87" s="2">
@@ -2748,7 +2755,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>120</v>
       </c>
@@ -2761,7 +2768,7 @@
       <c r="D88" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E88" s="2">
+      <c r="E88" s="3">
         <v>0.33928571428571425</v>
       </c>
       <c r="F88" s="2">
@@ -2774,7 +2781,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>120</v>
       </c>
@@ -2787,7 +2794,7 @@
       <c r="D89" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E89" s="2">
+      <c r="E89" s="3">
         <v>0.38297872340425532</v>
       </c>
       <c r="F89" s="2">
@@ -2800,7 +2807,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>120</v>
       </c>
@@ -2813,7 +2820,7 @@
       <c r="D90" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E90" s="2">
+      <c r="E90" s="3">
         <v>0.69230769230769229</v>
       </c>
       <c r="F90" s="2">
@@ -2826,7 +2833,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>120</v>
       </c>
@@ -2839,7 +2846,7 @@
       <c r="D91" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E91" s="2">
+      <c r="E91" s="3">
         <v>0.70833333333333337</v>
       </c>
       <c r="F91" s="2">
@@ -2852,7 +2859,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>120</v>
       </c>
@@ -2865,7 +2872,7 @@
       <c r="D92" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E92" s="2">
+      <c r="E92" s="3">
         <v>0.68085106382978733</v>
       </c>
       <c r="F92" s="2">
@@ -2878,7 +2885,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>120</v>
       </c>
@@ -2891,7 +2898,7 @@
       <c r="D93" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E93" s="2">
+      <c r="E93" s="3">
         <v>0.71698113207547165</v>
       </c>
       <c r="F93" s="2">
@@ -2904,7 +2911,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>120</v>
       </c>
@@ -2917,7 +2924,7 @@
       <c r="D94" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E94" s="2">
+      <c r="E94" s="3">
         <v>0.7</v>
       </c>
       <c r="F94" s="2">
@@ -2930,7 +2937,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>120</v>
       </c>
@@ -2943,7 +2950,7 @@
       <c r="D95" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E95" s="2">
+      <c r="E95" s="3">
         <v>0.57446808510638303</v>
       </c>
       <c r="F95" s="2">
@@ -2956,7 +2963,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>120</v>
       </c>
@@ -2969,7 +2976,7 @@
       <c r="D96" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E96" s="2">
+      <c r="E96" s="3">
         <v>0.72340425531914898</v>
       </c>
       <c r="F96" s="2">
@@ -2982,7 +2989,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>120</v>
       </c>
@@ -2995,7 +3002,7 @@
       <c r="D97" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E97" s="2">
+      <c r="E97" s="3">
         <v>0.64285714285714279</v>
       </c>
       <c r="F97" s="2">
@@ -3008,7 +3015,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>120</v>
       </c>
@@ -3021,7 +3028,7 @@
       <c r="D98" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E98" s="2">
+      <c r="E98" s="3">
         <v>0.60465116279069764</v>
       </c>
       <c r="F98" s="2">
@@ -3034,7 +3041,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>120</v>
       </c>
@@ -3047,7 +3054,7 @@
       <c r="D99" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E99" s="2">
+      <c r="E99" s="3">
         <v>0.67441860465116277</v>
       </c>
       <c r="F99" s="2">
@@ -3060,7 +3067,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>120</v>
       </c>
@@ -3073,7 +3080,7 @@
       <c r="D100" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E100" s="2">
+      <c r="E100" s="3">
         <v>0.87179487179487181</v>
       </c>
       <c r="F100" s="2">
@@ -3086,7 +3093,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>120</v>
       </c>
@@ -3099,7 +3106,7 @@
       <c r="D101" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E101" s="2">
+      <c r="E101" s="3">
         <v>0.97777777777777775</v>
       </c>
       <c r="F101" s="2">
@@ -3112,7 +3119,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>120</v>
       </c>
@@ -3125,7 +3132,7 @@
       <c r="D102" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E102" s="2">
+      <c r="E102" s="3">
         <v>0.93181818181818188</v>
       </c>
       <c r="F102" s="2">
@@ -3138,7 +3145,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>120</v>
       </c>
@@ -3151,7 +3158,7 @@
       <c r="D103" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E103" s="2">
+      <c r="E103" s="3">
         <v>0.95555555555555549</v>
       </c>
       <c r="F103" s="2">
@@ -3164,7 +3171,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>120</v>
       </c>
@@ -3177,7 +3184,7 @@
       <c r="D104" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E104" s="2">
+      <c r="E104" s="3">
         <v>0.97826086956521741</v>
       </c>
       <c r="F104" s="2">
@@ -3190,7 +3197,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>120</v>
       </c>
@@ -3203,7 +3210,7 @@
       <c r="D105" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E105" s="2">
+      <c r="E105" s="3">
         <v>0.97916666666666663</v>
       </c>
       <c r="F105" s="2">
@@ -3216,7 +3223,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>120</v>
       </c>
@@ -3229,7 +3236,7 @@
       <c r="D106" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E106" s="2">
+      <c r="E106" s="3">
         <v>0.42424242424242425</v>
       </c>
       <c r="F106" s="2">
@@ -3242,7 +3249,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>120</v>
       </c>
@@ -3255,7 +3262,7 @@
       <c r="D107" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E107" s="2">
+      <c r="E107" s="3">
         <v>0.25714285714285717</v>
       </c>
       <c r="F107" s="2">
@@ -3268,7 +3275,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>120</v>
       </c>
@@ -3281,7 +3288,7 @@
       <c r="D108" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E108" s="2">
+      <c r="E108" s="3">
         <v>0.17241379310344829</v>
       </c>
       <c r="F108" s="2">
@@ -3294,7 +3301,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>120</v>
       </c>
@@ -3307,7 +3314,7 @@
       <c r="D109" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E109" s="2">
+      <c r="E109" s="3">
         <v>0.23333333333333331</v>
       </c>
       <c r="F109" s="2">
@@ -3320,7 +3327,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>120</v>
       </c>
@@ -3333,7 +3340,7 @@
       <c r="D110" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E110" s="2">
+      <c r="E110" s="3">
         <v>0.4137931034482758</v>
       </c>
       <c r="F110" s="2">
@@ -3346,7 +3353,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>120</v>
       </c>
@@ -3359,7 +3366,7 @@
       <c r="D111" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E111" s="2">
+      <c r="E111" s="3">
         <v>0.41935483870967744</v>
       </c>
       <c r="F111" s="2">
@@ -3372,7 +3379,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>120</v>
       </c>
@@ -3385,7 +3392,7 @@
       <c r="D112" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E112" s="2">
+      <c r="E112" s="3">
         <v>0.32500000000000001</v>
       </c>
       <c r="F112" s="2">
@@ -3398,7 +3405,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>120</v>
       </c>
@@ -3411,7 +3418,7 @@
       <c r="D113" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E113" s="2">
+      <c r="E113" s="3">
         <v>0.35294117647058826</v>
       </c>
       <c r="F113" s="2">
@@ -3424,7 +3431,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>120</v>
       </c>
@@ -3437,7 +3444,7 @@
       <c r="D114" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E114" s="2">
+      <c r="E114" s="3">
         <v>0.5</v>
       </c>
       <c r="F114" s="2">
@@ -3450,7 +3457,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>120</v>
       </c>
@@ -3463,7 +3470,7 @@
       <c r="D115" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E115" s="2">
+      <c r="E115" s="3">
         <v>0.7142857142857143</v>
       </c>
       <c r="F115" s="2">
@@ -3476,7 +3483,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>120</v>
       </c>
@@ -3489,7 +3496,7 @@
       <c r="D116" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E116" s="2">
+      <c r="E116" s="3">
         <v>0.68421052631578949</v>
       </c>
       <c r="F116" s="2">
@@ -3502,7 +3509,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>120</v>
       </c>
@@ -3515,7 +3522,7 @@
       <c r="D117" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E117" s="2">
+      <c r="E117" s="3">
         <v>0.36734693877551022</v>
       </c>
       <c r="F117" s="2">
@@ -3528,7 +3535,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>120</v>
       </c>
@@ -3541,7 +3548,7 @@
       <c r="D118" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E118" s="2">
+      <c r="E118" s="3">
         <v>0.63888888888888895</v>
       </c>
       <c r="F118" s="2">
@@ -3554,7 +3561,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>120</v>
       </c>
@@ -3567,7 +3574,7 @@
       <c r="D119" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E119" s="2">
+      <c r="E119" s="3">
         <v>0.5576923076923076</v>
       </c>
       <c r="F119" s="2">
@@ -3580,7 +3587,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>120</v>
       </c>
@@ -3593,7 +3600,7 @@
       <c r="D120" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E120" s="2">
+      <c r="E120" s="3">
         <v>0.57499999999999996</v>
       </c>
       <c r="F120" s="2">
@@ -3606,7 +3613,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>120</v>
       </c>
@@ -3619,7 +3626,7 @@
       <c r="D121" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E121" s="2">
+      <c r="E121" s="3">
         <v>0.8529411764705882</v>
       </c>
       <c r="F121" s="2">
@@ -3632,7 +3639,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>120</v>
       </c>
@@ -3645,7 +3652,7 @@
       <c r="D122" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E122" s="2">
+      <c r="E122" s="3">
         <v>0.65</v>
       </c>
       <c r="F122" s="2">
@@ -3658,7 +3665,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>120</v>
       </c>
@@ -3671,7 +3678,7 @@
       <c r="D123" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E123" s="2">
+      <c r="E123" s="3">
         <v>0.61764705882352944</v>
       </c>
       <c r="F123" s="2">
@@ -3684,7 +3691,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>120</v>
       </c>
@@ -3697,7 +3704,7 @@
       <c r="D124" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E124" s="2">
+      <c r="E124" s="3">
         <v>0.58695652173913049</v>
       </c>
       <c r="F124" s="2">
@@ -3710,7 +3717,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>120</v>
       </c>
@@ -3723,7 +3730,7 @@
       <c r="D125" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E125" s="2">
+      <c r="E125" s="3">
         <v>0.84375</v>
       </c>
       <c r="F125" s="2">
@@ -3736,7 +3743,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>120</v>
       </c>
@@ -3749,7 +3756,7 @@
       <c r="D126" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E126" s="2">
+      <c r="E126" s="3">
         <v>0.93333333333333335</v>
       </c>
       <c r="F126" s="2">
@@ -3762,7 +3769,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>120</v>
       </c>
@@ -3775,7 +3782,7 @@
       <c r="D127" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E127" s="2">
+      <c r="E127" s="3">
         <v>0.97916666666666663</v>
       </c>
       <c r="F127" s="2">
@@ -3788,7 +3795,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>120</v>
       </c>
@@ -3801,7 +3808,7 @@
       <c r="D128" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E128" s="2">
+      <c r="E128" s="3">
         <v>1</v>
       </c>
       <c r="F128" s="2">
@@ -3814,7 +3821,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>120</v>
       </c>
@@ -3827,7 +3834,7 @@
       <c r="D129" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E129" s="2">
+      <c r="E129" s="3">
         <v>0.97297297297297292</v>
       </c>
       <c r="F129" s="2">
@@ -3840,7 +3847,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>120</v>
       </c>
@@ -3853,7 +3860,7 @@
       <c r="D130" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E130" s="2">
+      <c r="E130" s="3">
         <v>1</v>
       </c>
       <c r="F130" s="2">
@@ -3866,7 +3873,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>120</v>
       </c>
@@ -3879,7 +3886,7 @@
       <c r="D131" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E131" s="2">
+      <c r="E131" s="3">
         <v>0.85135135135134987</v>
       </c>
       <c r="F131" s="2">
@@ -3892,7 +3899,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>120</v>
       </c>
@@ -3905,7 +3912,7 @@
       <c r="D132" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E132" s="2">
+      <c r="E132" s="3">
         <v>0.79019073569482123</v>
       </c>
       <c r="F132" s="2">
@@ -3918,7 +3925,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <v>120</v>
       </c>
@@ -3931,7 +3938,7 @@
       <c r="D133" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E133" s="2">
+      <c r="E133" s="3">
         <v>0.84024896265560045</v>
       </c>
       <c r="F133" s="2">
@@ -3944,7 +3951,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>120</v>
       </c>
@@ -3957,7 +3964,7 @@
       <c r="D134" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E134" s="2">
+      <c r="E134" s="3">
         <v>0.90517241379310254</v>
       </c>
       <c r="F134" s="2">
@@ -3970,7 +3977,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <v>120</v>
       </c>
@@ -3983,7 +3990,7 @@
       <c r="D135" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E135" s="2">
+      <c r="E135" s="3">
         <v>0.74712643678160728</v>
       </c>
       <c r="F135" s="2">
@@ -3996,7 +4003,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <v>120</v>
       </c>
@@ -4009,7 +4016,7 @@
       <c r="D136" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E136" s="2">
+      <c r="E136" s="3">
         <v>0.61991869918698905</v>
       </c>
       <c r="F136" s="2">
@@ -4022,7 +4029,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>120</v>
       </c>
@@ -4035,7 +4042,7 @@
       <c r="D137" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E137" s="2">
+      <c r="E137" s="3">
         <v>0.74918566775244155</v>
       </c>
       <c r="F137" s="2">
@@ -4048,7 +4055,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>120</v>
       </c>
@@ -4061,7 +4068,7 @@
       <c r="D138" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E138" s="2">
+      <c r="E138" s="3">
         <v>0.64920273348519086</v>
       </c>
       <c r="F138" s="2">
@@ -4074,7 +4081,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <v>120</v>
       </c>
@@ -4087,7 +4094,7 @@
       <c r="D139" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E139" s="2">
+      <c r="E139" s="3">
         <v>0.86278586278586178</v>
       </c>
       <c r="F139" s="2">
@@ -4100,7 +4107,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>120</v>
       </c>
@@ -4113,7 +4120,7 @@
       <c r="D140" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E140" s="2">
+      <c r="E140" s="3">
         <v>0.68143100511073029</v>
       </c>
       <c r="F140" s="2">
@@ -4126,7 +4133,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <v>120</v>
       </c>
@@ -4139,7 +4146,7 @@
       <c r="D141" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E141" s="2">
+      <c r="E141" s="3">
         <v>0.88640275387263268</v>
       </c>
       <c r="F141" s="2">
@@ -4152,7 +4159,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <v>120</v>
       </c>
@@ -4165,7 +4172,7 @@
       <c r="D142" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E142" s="2">
+      <c r="E142" s="3">
         <v>0.88098918083462063</v>
       </c>
       <c r="F142" s="2">
@@ -4178,7 +4185,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <v>120</v>
       </c>
@@ -4191,7 +4198,7 @@
       <c r="D143" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E143" s="2">
+      <c r="E143" s="3">
         <v>0.93004769475357674</v>
       </c>
       <c r="F143" s="2">
@@ -4204,7 +4211,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
         <v>120</v>
       </c>
@@ -4217,7 +4224,7 @@
       <c r="D144" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E144" s="2">
+      <c r="E144" s="3">
         <v>0.86230876216967955</v>
       </c>
       <c r="F144" s="2">
@@ -4230,7 +4237,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <v>120</v>
       </c>
@@ -4243,7 +4250,7 @@
       <c r="D145" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E145" s="2">
+      <c r="E145" s="3">
         <v>0.86134453781512521</v>
       </c>
       <c r="F145" s="2">
@@ -4256,7 +4263,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>120</v>
       </c>
@@ -4269,7 +4276,7 @@
       <c r="D146" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E146" s="2">
+      <c r="E146" s="3">
         <v>0.92872570194384396</v>
       </c>
       <c r="F146" s="2">
@@ -4282,7 +4289,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <v>120</v>
       </c>
@@ -4295,7 +4302,7 @@
       <c r="D147" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E147" s="2">
+      <c r="E147" s="3">
         <v>0.88999999999999913</v>
       </c>
       <c r="F147" s="2">
@@ -4308,7 +4315,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>120</v>
       </c>
@@ -4321,7 +4328,7 @@
       <c r="D148" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E148" s="2">
+      <c r="E148" s="3">
         <v>0.94827586206896519</v>
       </c>
       <c r="F148" s="2">
@@ -4334,7 +4341,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <v>120</v>
       </c>
@@ -4347,7 +4354,7 @@
       <c r="D149" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E149" s="2">
+      <c r="E149" s="3">
         <v>0.92775041050903084</v>
       </c>
       <c r="F149" s="2">
@@ -4360,7 +4367,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <v>120</v>
       </c>
@@ -4373,7 +4380,7 @@
       <c r="D150" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E150" s="2">
+      <c r="E150" s="3">
         <v>0.90983606557376995</v>
       </c>
       <c r="F150" s="2">
@@ -4386,7 +4393,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
         <v>120</v>
       </c>
@@ -4399,7 +4406,7 @@
       <c r="D151" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E151" s="2">
+      <c r="E151" s="3">
         <v>0.96491228070175417</v>
       </c>
       <c r="F151" s="2">
@@ -4412,7 +4419,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <v>120</v>
       </c>
@@ -4425,7 +4432,7 @@
       <c r="D152" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E152" s="2">
+      <c r="E152" s="3">
         <v>0.95990279465370576</v>
       </c>
       <c r="F152" s="2">
@@ -4438,7 +4445,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
         <v>120</v>
       </c>
@@ -4451,7 +4458,7 @@
       <c r="D153" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E153" s="2">
+      <c r="E153" s="3">
         <v>0.94703049759229496</v>
       </c>
       <c r="F153" s="2">
@@ -4464,7 +4471,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
         <v>120</v>
       </c>
@@ -4477,7 +4484,7 @@
       <c r="D154" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E154" s="2">
+      <c r="E154" s="3">
         <v>0.98408104196816204</v>
       </c>
       <c r="F154" s="2">
@@ -4490,7 +4497,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
         <v>120</v>
       </c>
@@ -4503,7 +4510,7 @@
       <c r="D155" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E155" s="2">
+      <c r="E155" s="3">
         <v>1</v>
       </c>
       <c r="F155" s="2">
@@ -4516,7 +4523,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
         <v>158</v>
       </c>
@@ -4529,7 +4536,7 @@
       <c r="D156" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E156" s="1">
+      <c r="E156" s="3">
         <v>1</v>
       </c>
       <c r="F156" s="1">
@@ -4539,7 +4546,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
         <v>158</v>
       </c>
@@ -4552,7 +4559,7 @@
       <c r="D157" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E157" s="1">
+      <c r="E157" s="3">
         <v>1</v>
       </c>
       <c r="F157" s="1">
@@ -4562,7 +4569,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
         <v>158</v>
       </c>
@@ -4575,7 +4582,7 @@
       <c r="D158" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E158" s="1">
+      <c r="E158" s="3">
         <v>0</v>
       </c>
       <c r="F158" s="1">
@@ -4585,7 +4592,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
         <v>158</v>
       </c>
@@ -4598,7 +4605,7 @@
       <c r="D159" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E159" s="1">
+      <c r="E159" s="3">
         <v>1</v>
       </c>
       <c r="F159" s="1">
@@ -4608,7 +4615,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
         <v>158</v>
       </c>
@@ -4621,7 +4628,7 @@
       <c r="D160" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E160" s="1">
+      <c r="E160" s="3">
         <v>1</v>
       </c>
       <c r="F160" s="1">
@@ -4631,7 +4638,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
         <v>158</v>
       </c>
@@ -4644,7 +4651,7 @@
       <c r="D161" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E161" s="1">
+      <c r="E161" s="3">
         <v>0</v>
       </c>
       <c r="F161" s="1">
@@ -4654,7 +4661,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
         <v>158</v>
       </c>
@@ -4667,7 +4674,7 @@
       <c r="D162" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E162" s="1">
+      <c r="E162" s="3">
         <v>1</v>
       </c>
       <c r="F162" s="1">
@@ -4677,7 +4684,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
         <v>158</v>
       </c>
@@ -4690,7 +4697,7 @@
       <c r="D163" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E163" s="1">
+      <c r="E163" s="3">
         <v>0</v>
       </c>
       <c r="F163" s="1">
@@ -4700,7 +4707,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
         <v>158</v>
       </c>
@@ -4713,7 +4720,7 @@
       <c r="D164" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E164" s="1">
+      <c r="E164" s="3">
         <v>0</v>
       </c>
       <c r="F164" s="1">
@@ -4723,7 +4730,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
         <v>158</v>
       </c>
@@ -4736,7 +4743,7 @@
       <c r="D165" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E165" s="1">
+      <c r="E165" s="3">
         <v>1</v>
       </c>
       <c r="F165" s="1">
@@ -4746,7 +4753,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
         <v>158</v>
       </c>
@@ -4759,7 +4766,7 @@
       <c r="D166" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E166" s="1">
+      <c r="E166" s="3">
         <v>4</v>
       </c>
       <c r="F166" s="1">
@@ -4769,7 +4776,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
         <v>158</v>
       </c>
@@ -4782,7 +4789,7 @@
       <c r="D167" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E167" s="1">
+      <c r="E167" s="3">
         <v>5</v>
       </c>
       <c r="F167" s="1">
@@ -4792,7 +4799,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
         <v>158</v>
       </c>
@@ -4805,7 +4812,7 @@
       <c r="D168" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E168" s="1">
+      <c r="E168" s="3">
         <v>2</v>
       </c>
       <c r="F168" s="1">
@@ -4815,7 +4822,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
         <v>158</v>
       </c>
@@ -4828,7 +4835,7 @@
       <c r="D169" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E169" s="1">
+      <c r="E169" s="3">
         <v>5</v>
       </c>
       <c r="F169" s="1">
@@ -4838,7 +4845,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
         <v>158</v>
       </c>
@@ -4851,7 +4858,7 @@
       <c r="D170" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E170" s="1">
+      <c r="E170" s="3">
         <v>4</v>
       </c>
       <c r="F170" s="1">
@@ -4861,7 +4868,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
         <v>158</v>
       </c>
@@ -4874,7 +4881,7 @@
       <c r="D171" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E171" s="1">
+      <c r="E171" s="3">
         <v>1</v>
       </c>
       <c r="F171" s="1">
@@ -4884,7 +4891,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
         <v>158</v>
       </c>
@@ -4897,7 +4904,7 @@
       <c r="D172" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E172" s="1">
+      <c r="E172" s="3">
         <v>1</v>
       </c>
       <c r="F172" s="1">
@@ -4907,7 +4914,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
         <v>158</v>
       </c>
@@ -4920,7 +4927,7 @@
       <c r="D173" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E173" s="1">
+      <c r="E173" s="3">
         <v>3</v>
       </c>
       <c r="F173" s="1">
@@ -4930,7 +4937,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
         <v>158</v>
       </c>
@@ -4943,7 +4950,7 @@
       <c r="D174" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E174" s="1">
+      <c r="E174" s="3">
         <v>1</v>
       </c>
       <c r="F174" s="1">
@@ -4953,7 +4960,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
         <v>158</v>
       </c>
@@ -4966,7 +4973,7 @@
       <c r="D175" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E175" s="1">
+      <c r="E175" s="3">
         <v>2</v>
       </c>
       <c r="F175" s="1">
@@ -4976,7 +4983,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
         <v>158</v>
       </c>
@@ -4989,7 +4996,7 @@
       <c r="D176" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E176" s="1">
+      <c r="E176" s="3">
         <v>2</v>
       </c>
       <c r="F176" s="1">
@@ -4999,7 +5006,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
         <v>158</v>
       </c>
@@ -5012,7 +5019,7 @@
       <c r="D177" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E177" s="1">
+      <c r="E177" s="3">
         <v>7</v>
       </c>
       <c r="F177" s="1">
@@ -5022,7 +5029,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
         <v>158</v>
       </c>
@@ -5035,7 +5042,7 @@
       <c r="D178" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E178" s="1">
+      <c r="E178" s="3">
         <v>10</v>
       </c>
       <c r="F178" s="1">
@@ -5045,7 +5052,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
         <v>158</v>
       </c>
@@ -5058,7 +5065,7 @@
       <c r="D179" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E179" s="1">
+      <c r="E179" s="3">
         <v>10</v>
       </c>
       <c r="F179" s="1">
@@ -5068,7 +5075,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A180" s="1">
         <v>158</v>
       </c>
@@ -5081,7 +5088,7 @@
       <c r="D180" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E180" s="1">
+      <c r="E180" s="3">
         <v>2</v>
       </c>
       <c r="F180" s="1">
@@ -5091,7 +5098,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A181" s="1">
         <v>158</v>
       </c>
@@ -5104,7 +5111,7 @@
       <c r="D181" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E181" s="1">
+      <c r="E181" s="3">
         <v>2</v>
       </c>
       <c r="F181" s="1">
@@ -5114,7 +5121,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A182" s="1">
         <v>158</v>
       </c>
@@ -5127,7 +5134,7 @@
       <c r="D182" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E182" s="1">
+      <c r="E182" s="3">
         <v>2</v>
       </c>
       <c r="F182" s="1">
@@ -5137,7 +5144,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A183" s="1">
         <v>158</v>
       </c>
@@ -5150,7 +5157,7 @@
       <c r="D183" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E183" s="1">
+      <c r="E183" s="3">
         <v>2</v>
       </c>
       <c r="F183" s="1">
@@ -5160,7 +5167,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
         <v>158</v>
       </c>
@@ -5173,7 +5180,7 @@
       <c r="D184" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E184" s="1">
+      <c r="E184" s="3">
         <v>5</v>
       </c>
       <c r="F184" s="1">
@@ -5183,7 +5190,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
         <v>158</v>
       </c>
@@ -5196,7 +5203,7 @@
       <c r="D185" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E185" s="1">
+      <c r="E185" s="3">
         <v>6</v>
       </c>
       <c r="F185" s="1">
@@ -5206,7 +5213,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A186" s="1">
         <v>158</v>
       </c>
@@ -5219,7 +5226,7 @@
       <c r="D186" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E186" s="1">
+      <c r="E186" s="3">
         <v>7</v>
       </c>
       <c r="F186" s="1">
@@ -5229,7 +5236,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
         <v>158</v>
       </c>
@@ -5242,7 +5249,7 @@
       <c r="D187" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E187" s="1">
+      <c r="E187" s="3">
         <v>10</v>
       </c>
       <c r="F187" s="1">
@@ -5252,7 +5259,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A188" s="1">
         <v>158</v>
       </c>
@@ -5265,7 +5272,7 @@
       <c r="D188" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E188" s="1">
+      <c r="E188" s="3">
         <v>10</v>
       </c>
       <c r="F188" s="1">
@@ -5275,7 +5282,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A189" s="1">
         <v>158</v>
       </c>
@@ -5288,7 +5295,7 @@
       <c r="D189" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E189" s="1">
+      <c r="E189" s="3">
         <v>1</v>
       </c>
       <c r="F189" s="1">
@@ -5298,7 +5305,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A190" s="1">
         <v>158</v>
       </c>
@@ -5311,7 +5318,7 @@
       <c r="D190" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E190" s="1">
+      <c r="E190" s="3">
         <v>0</v>
       </c>
       <c r="F190" s="1">
@@ -5321,7 +5328,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A191" s="1">
         <v>158</v>
       </c>
@@ -5334,7 +5341,7 @@
       <c r="D191" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E191" s="1">
+      <c r="E191" s="3">
         <v>0</v>
       </c>
       <c r="F191" s="1">
@@ -5344,7 +5351,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A192" s="1">
         <v>158</v>
       </c>
@@ -5357,7 +5364,7 @@
       <c r="D192" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E192" s="1">
+      <c r="E192" s="3">
         <v>1</v>
       </c>
       <c r="F192" s="1">
@@ -5367,7 +5374,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="193" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A193" s="1">
         <v>158</v>
       </c>
@@ -5380,7 +5387,7 @@
       <c r="D193" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E193" s="1">
+      <c r="E193" s="3">
         <v>0</v>
       </c>
       <c r="F193" s="1">
@@ -5390,7 +5397,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="194" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A194" s="1">
         <v>158</v>
       </c>
@@ -5403,7 +5410,7 @@
       <c r="D194" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E194" s="1">
+      <c r="E194" s="3">
         <v>0</v>
       </c>
       <c r="F194" s="1">
@@ -5413,7 +5420,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="195" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A195" s="1">
         <v>158</v>
       </c>
@@ -5426,7 +5433,7 @@
       <c r="D195" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E195" s="1">
+      <c r="E195" s="3">
         <v>1</v>
       </c>
       <c r="F195" s="1">
@@ -5436,7 +5443,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="196" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A196" s="1">
         <v>158</v>
       </c>
@@ -5449,7 +5456,7 @@
       <c r="D196" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E196" s="1">
+      <c r="E196" s="3">
         <v>1</v>
       </c>
       <c r="F196" s="1">
@@ -5459,7 +5466,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="197" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A197" s="1">
         <v>158</v>
       </c>
@@ -5472,7 +5479,7 @@
       <c r="D197" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E197" s="1">
+      <c r="E197" s="3">
         <v>4</v>
       </c>
       <c r="F197" s="1">
@@ -5482,7 +5489,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="198" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A198" s="1">
         <v>158</v>
       </c>
@@ -5495,7 +5502,7 @@
       <c r="D198" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E198" s="1">
+      <c r="E198" s="3">
         <v>6</v>
       </c>
       <c r="F198" s="1">
@@ -5505,7 +5512,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="199" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A199" s="1">
         <v>158</v>
       </c>
@@ -5518,7 +5525,7 @@
       <c r="D199" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E199" s="1">
+      <c r="E199" s="3">
         <v>6</v>
       </c>
       <c r="F199" s="1">
@@ -5528,7 +5535,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="200" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A200" s="1">
         <v>158</v>
       </c>
@@ -5541,7 +5548,7 @@
       <c r="D200" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E200" s="1">
+      <c r="E200" s="3">
         <v>5</v>
       </c>
       <c r="F200" s="1">
@@ -5551,7 +5558,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="201" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A201" s="1">
         <v>158</v>
       </c>
@@ -5564,7 +5571,7 @@
       <c r="D201" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E201" s="1">
+      <c r="E201" s="3">
         <v>5</v>
       </c>
       <c r="F201" s="1">
@@ -5574,7 +5581,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="202" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A202" s="1">
         <v>158</v>
       </c>
@@ -5587,7 +5594,7 @@
       <c r="D202" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E202" s="1">
+      <c r="E202" s="3">
         <v>3</v>
       </c>
       <c r="F202" s="1">
@@ -5597,263 +5604,263 @@
         <v>21</v>
       </c>
     </row>
-    <row r="217" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="217" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E217" s="2"/>
       <c r="F217" s="2"/>
     </row>
-    <row r="218" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="218" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E218" s="2"/>
       <c r="F218" s="2"/>
     </row>
-    <row r="219" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="219" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E219" s="2"/>
       <c r="F219" s="2"/>
     </row>
-    <row r="220" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="220" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E220" s="2"/>
       <c r="F220" s="2"/>
     </row>
-    <row r="221" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="221" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E221" s="2"/>
       <c r="F221" s="2"/>
     </row>
-    <row r="222" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="222" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E222" s="2"/>
       <c r="F222" s="2"/>
     </row>
-    <row r="223" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="223" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E223" s="2"/>
       <c r="F223" s="2"/>
     </row>
-    <row r="224" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="224" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E224" s="2"/>
       <c r="F224" s="2"/>
     </row>
-    <row r="225" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="225" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E225" s="2"/>
       <c r="F225" s="2"/>
     </row>
-    <row r="226" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="226" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E226" s="2"/>
       <c r="F226" s="2"/>
     </row>
-    <row r="227" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="227" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E227" s="2"/>
       <c r="F227" s="2"/>
     </row>
-    <row r="228" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="228" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E228" s="2"/>
       <c r="F228" s="2"/>
     </row>
-    <row r="229" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="229" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E229" s="2"/>
       <c r="F229" s="2"/>
     </row>
-    <row r="230" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="230" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E230" s="2"/>
       <c r="F230" s="2"/>
     </row>
-    <row r="231" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="231" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E231" s="2"/>
       <c r="F231" s="2"/>
     </row>
-    <row r="232" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="232" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E232" s="2"/>
       <c r="F232" s="2"/>
     </row>
-    <row r="233" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="233" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E233" s="2"/>
       <c r="F233" s="2"/>
     </row>
-    <row r="234" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="234" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E234" s="2"/>
       <c r="F234" s="2"/>
     </row>
-    <row r="235" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="235" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E235" s="2"/>
       <c r="F235" s="2"/>
     </row>
-    <row r="236" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="236" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E236" s="2"/>
       <c r="F236" s="2"/>
     </row>
-    <row r="237" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="237" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E237" s="2"/>
       <c r="F237" s="2"/>
     </row>
-    <row r="238" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="238" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E238" s="2"/>
       <c r="F238" s="2"/>
     </row>
-    <row r="239" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="239" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E239" s="2"/>
       <c r="F239" s="2"/>
     </row>
-    <row r="240" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="240" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E240" s="2"/>
       <c r="F240" s="2"/>
     </row>
-    <row r="241" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="241" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E241" s="2"/>
       <c r="F241" s="2"/>
     </row>
-    <row r="289" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="289" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E289" s="2"/>
       <c r="F289" s="2"/>
     </row>
-    <row r="290" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="290" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E290" s="2"/>
       <c r="F290" s="2"/>
     </row>
-    <row r="291" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="291" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E291" s="2"/>
       <c r="F291" s="2"/>
     </row>
-    <row r="292" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="292" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E292" s="2"/>
       <c r="F292" s="2"/>
     </row>
-    <row r="293" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="293" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E293" s="2"/>
       <c r="F293" s="2"/>
     </row>
-    <row r="294" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="294" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E294" s="2"/>
       <c r="F294" s="2"/>
     </row>
-    <row r="295" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="295" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E295" s="2"/>
       <c r="F295" s="2"/>
     </row>
-    <row r="296" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="296" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E296" s="2"/>
       <c r="F296" s="2"/>
     </row>
-    <row r="297" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="297" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E297" s="2"/>
       <c r="F297" s="2"/>
     </row>
-    <row r="298" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="298" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E298" s="2"/>
       <c r="F298" s="2"/>
     </row>
-    <row r="299" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="299" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E299" s="2"/>
       <c r="F299" s="2"/>
     </row>
-    <row r="300" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="300" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E300" s="2"/>
       <c r="F300" s="2"/>
     </row>
-    <row r="301" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="301" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E301" s="2"/>
       <c r="F301" s="2"/>
     </row>
-    <row r="302" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="302" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E302" s="2"/>
       <c r="F302" s="2"/>
     </row>
-    <row r="303" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="303" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E303" s="2"/>
       <c r="F303" s="2"/>
     </row>
-    <row r="304" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="304" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E304" s="2"/>
       <c r="F304" s="2"/>
     </row>
-    <row r="305" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="305" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E305" s="2"/>
       <c r="F305" s="2"/>
     </row>
-    <row r="306" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="306" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E306" s="2"/>
       <c r="F306" s="2"/>
     </row>
-    <row r="307" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="307" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E307" s="2"/>
       <c r="F307" s="2"/>
     </row>
-    <row r="308" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="308" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E308" s="2"/>
       <c r="F308" s="2"/>
     </row>
-    <row r="309" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="309" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E309" s="2"/>
       <c r="F309" s="2"/>
     </row>
-    <row r="310" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="310" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E310" s="2"/>
       <c r="F310" s="2"/>
     </row>
-    <row r="311" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="311" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E311" s="2"/>
       <c r="F311" s="2"/>
     </row>
-    <row r="312" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="312" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E312" s="2"/>
       <c r="F312" s="2"/>
     </row>
-    <row r="313" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="313" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E313" s="2"/>
       <c r="F313" s="2"/>
     </row>
-    <row r="314" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="314" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E314" s="2"/>
       <c r="F314" s="2"/>
     </row>
-    <row r="315" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="315" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E315" s="2"/>
       <c r="F315" s="2"/>
     </row>
-    <row r="316" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="316" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E316" s="2"/>
       <c r="F316" s="2"/>
     </row>
-    <row r="317" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="317" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E317" s="2"/>
       <c r="F317" s="2"/>
     </row>
-    <row r="318" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="318" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E318" s="2"/>
       <c r="F318" s="2"/>
     </row>
-    <row r="319" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="319" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E319" s="2"/>
       <c r="F319" s="2"/>
     </row>
-    <row r="320" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="320" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E320" s="2"/>
       <c r="F320" s="2"/>
     </row>
-    <row r="321" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="321" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E321" s="2"/>
       <c r="F321" s="2"/>
     </row>
-    <row r="322" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="322" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E322" s="2"/>
       <c r="F322" s="2"/>
     </row>
-    <row r="323" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="323" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E323" s="2"/>
       <c r="F323" s="2"/>
     </row>
-    <row r="324" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="324" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E324" s="2"/>
       <c r="F324" s="2"/>
     </row>
-    <row r="325" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="325" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E325" s="2"/>
       <c r="F325" s="2"/>
     </row>
-    <row r="326" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="326" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E326" s="2"/>
       <c r="F326" s="2"/>
     </row>
-    <row r="327" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="327" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E327" s="2"/>
       <c r="F327" s="2"/>
     </row>
-    <row r="328" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="328" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E328" s="2"/>
       <c r="F328" s="2"/>
     </row>

</xml_diff>